<commit_message>
Update progbooks to add units
</commit_message>
<xml_diff>
--- a/tests/databooks/progbook_hypertension.xlsx
+++ b/tests/databooks/progbook_hypertension.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="43">
   <si>
     <t>Targeted to (populations)</t>
   </si>
@@ -78,13 +78,19 @@
     <t>Adherence</t>
   </si>
   <si>
+    <t>Units</t>
+  </si>
+  <si>
     <t>Uncertainty</t>
   </si>
   <si>
     <t>Assumption</t>
   </si>
   <si>
-    <t>Total spend</t>
+    <t>Annual spend</t>
+  </si>
+  <si>
+    <t>$/year</t>
   </si>
   <si>
     <t>OR</t>
@@ -93,12 +99,21 @@
     <t>Unit cost</t>
   </si>
   <si>
+    <t>$/person</t>
+  </si>
+  <si>
     <t>Capacity</t>
   </si>
   <si>
+    <t>people/year</t>
+  </si>
+  <si>
     <t>Saturation</t>
   </si>
   <si>
+    <t>N.A.</t>
+  </si>
+  <si>
     <t>Coverage</t>
   </si>
   <si>
@@ -114,7 +129,7 @@
     <t>Impact interaction</t>
   </si>
   <si>
-    <t>additive</t>
+    <t>Additive</t>
   </si>
   <si>
     <t>best</t>
@@ -1176,7 +1191,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1184,13 +1199,15 @@
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="3.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="2" t="s">
-        <v>13</v>
+    <row r="1" spans="1:9">
+      <c r="A1" s="2" t="str">
+        <f>'Program targeting'!$B$3</f>
+        <v>Screening - urban</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>20</v>
@@ -1198,99 +1215,118 @@
       <c r="C1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2">
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2">
         <v>2015</v>
       </c>
-      <c r="F1" s="2">
+      <c r="G1" s="2">
         <v>2016</v>
       </c>
-      <c r="G1" s="2">
+      <c r="H1" s="2">
         <v>2017</v>
       </c>
-      <c r="H1" s="2">
+      <c r="I1" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6">
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6">
         <v>21500</v>
       </c>
-      <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6">
         <v>72</v>
       </c>
-      <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
       <c r="C5" s="5"/>
-      <c r="D5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6">
         <v>298.6111111111111</v>
       </c>
-      <c r="G6" s="6"/>
       <c r="H6" s="6"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="2" t="s">
-        <v>16</v>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="2" t="str">
+        <f>'Program targeting'!$B$4</f>
+        <v>Screening - rural</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>20</v>
@@ -1298,99 +1334,118 @@
       <c r="C8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2">
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2">
         <v>2015</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>2016</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>2017</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6">
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6">
         <v>32500</v>
       </c>
-      <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6">
         <v>108</v>
       </c>
-      <c r="G10" s="6"/>
       <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6">
         <v>300.925925925926</v>
       </c>
-      <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="2" t="s">
-        <v>17</v>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="2" t="str">
+        <f>'Program targeting'!$B$5</f>
+        <v>Confirmatory test</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>20</v>
@@ -1398,99 +1453,118 @@
       <c r="C15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2">
+      <c r="D15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2">
         <v>2015</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>2016</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>2017</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I15" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6">
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6">
         <v>1900</v>
       </c>
-      <c r="G16" s="6"/>
       <c r="H16" s="6"/>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6">
         <v>24</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6">
-        <v>24</v>
-      </c>
-      <c r="G17" s="6"/>
       <c r="H17" s="6"/>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
       <c r="C19" s="5"/>
-      <c r="D19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6">
         <v>79.16666666666667</v>
       </c>
-      <c r="G20" s="6"/>
       <c r="H20" s="6"/>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="2" t="s">
-        <v>18</v>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="2" t="str">
+        <f>'Program targeting'!$B$6</f>
+        <v>Treatment initiation</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>20</v>
@@ -1498,99 +1572,118 @@
       <c r="C22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2">
+      <c r="D22" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2">
         <v>2015</v>
       </c>
-      <c r="F22" s="2">
+      <c r="G22" s="2">
         <v>2016</v>
       </c>
-      <c r="G22" s="2">
+      <c r="H22" s="2">
         <v>2017</v>
       </c>
-      <c r="H22" s="2">
+      <c r="I22" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:9">
       <c r="A23" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6">
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6">
         <v>2500</v>
       </c>
-      <c r="G23" s="6"/>
       <c r="H23" s="6"/>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6">
         <v>45</v>
       </c>
-      <c r="G24" s="6"/>
       <c r="H24" s="6"/>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6">
+        <v>32</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6">
         <v>55.55555555555556</v>
       </c>
-      <c r="G27" s="6"/>
       <c r="H27" s="6"/>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="2" t="s">
-        <v>19</v>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="2" t="str">
+        <f>'Program targeting'!$B$7</f>
+        <v>Adherence</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>20</v>
@@ -1598,297 +1691,347 @@
       <c r="C29" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2">
+      <c r="D29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2">
         <v>2015</v>
       </c>
-      <c r="F29" s="2">
+      <c r="G29" s="2">
         <v>2016</v>
       </c>
-      <c r="G29" s="2">
+      <c r="H29" s="2">
         <v>2017</v>
       </c>
-      <c r="H29" s="2">
+      <c r="I29" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9">
       <c r="A30" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6">
+      <c r="B30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6">
         <v>4000</v>
       </c>
-      <c r="G30" s="6"/>
       <c r="H30" s="6"/>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6">
+        <v>26</v>
+      </c>
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6">
         <v>45</v>
       </c>
-      <c r="G31" s="6"/>
       <c r="H31" s="6"/>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="I31" s="6"/>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
+        <v>31</v>
+      </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6">
         <v>88.88888888888889</v>
       </c>
-      <c r="G34" s="6"/>
       <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C10">
     <cfRule type="expression" dxfId="1" priority="13">
-      <formula>COUNTIF(E10:H10,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F10:I10,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="14">
-      <formula>AND(COUNTIF(E10:H10,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C10)))</formula>
+      <formula>AND(COUNTIF(F10:I10,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
     <cfRule type="expression" dxfId="1" priority="15">
-      <formula>COUNTIF(E11:H11,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F11:I11,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="16">
-      <formula>AND(COUNTIF(E11:H11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C11)))</formula>
+      <formula>AND(COUNTIF(F11:I11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
     <cfRule type="expression" dxfId="1" priority="17">
-      <formula>COUNTIF(E12:H12,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F12:I12,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="18">
-      <formula>AND(COUNTIF(E12:H12,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C12)))</formula>
+      <formula>AND(COUNTIF(F12:I12,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
     <cfRule type="expression" dxfId="1" priority="19">
-      <formula>COUNTIF(E13:H13,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F13:I13,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="20">
-      <formula>AND(COUNTIF(E13:H13,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C13)))</formula>
+      <formula>AND(COUNTIF(F13:I13,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
     <cfRule type="expression" dxfId="1" priority="21">
-      <formula>COUNTIF(E16:H16,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F16:I16,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="22">
-      <formula>AND(COUNTIF(E16:H16,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C16)))</formula>
+      <formula>AND(COUNTIF(F16:I16,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
     <cfRule type="expression" dxfId="1" priority="23">
-      <formula>COUNTIF(E17:H17,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F17:I17,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="24">
-      <formula>AND(COUNTIF(E17:H17,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C17)))</formula>
+      <formula>AND(COUNTIF(F17:I17,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
     <cfRule type="expression" dxfId="1" priority="25">
-      <formula>COUNTIF(E18:H18,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F18:I18,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="26">
-      <formula>AND(COUNTIF(E18:H18,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C18)))</formula>
+      <formula>AND(COUNTIF(F18:I18,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
     <cfRule type="expression" dxfId="1" priority="27">
-      <formula>COUNTIF(E19:H19,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F19:I19,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="28">
-      <formula>AND(COUNTIF(E19:H19,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C19)))</formula>
+      <formula>AND(COUNTIF(F19:I19,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
     <cfRule type="expression" dxfId="1" priority="1">
-      <formula>COUNTIF(E2:H2,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F2:I2,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="2">
-      <formula>AND(COUNTIF(E2:H2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C2)))</formula>
+      <formula>AND(COUNTIF(F2:I2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
     <cfRule type="expression" dxfId="1" priority="29">
-      <formula>COUNTIF(E20:H20,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F20:I20,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="30">
-      <formula>AND(COUNTIF(E20:H20,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C20)))</formula>
+      <formula>AND(COUNTIF(F20:I20,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
     <cfRule type="expression" dxfId="1" priority="31">
-      <formula>COUNTIF(E23:H23,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F23:I23,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="32">
-      <formula>AND(COUNTIF(E23:H23,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C23)))</formula>
+      <formula>AND(COUNTIF(F23:I23,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
     <cfRule type="expression" dxfId="1" priority="33">
-      <formula>COUNTIF(E24:H24,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F24:I24,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="34">
-      <formula>AND(COUNTIF(E24:H24,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C24)))</formula>
+      <formula>AND(COUNTIF(F24:I24,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
     <cfRule type="expression" dxfId="1" priority="35">
-      <formula>COUNTIF(E25:H25,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F25:I25,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="36">
-      <formula>AND(COUNTIF(E25:H25,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C25)))</formula>
+      <formula>AND(COUNTIF(F25:I25,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
     <cfRule type="expression" dxfId="1" priority="37">
-      <formula>COUNTIF(E26:H26,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F26:I26,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="38">
-      <formula>AND(COUNTIF(E26:H26,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C26)))</formula>
+      <formula>AND(COUNTIF(F26:I26,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
     <cfRule type="expression" dxfId="1" priority="39">
-      <formula>COUNTIF(E27:H27,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F27:I27,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="40">
-      <formula>AND(COUNTIF(E27:H27,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C27)))</formula>
+      <formula>AND(COUNTIF(F27:I27,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
     <cfRule type="expression" dxfId="1" priority="3">
-      <formula>COUNTIF(E3:H3,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F3:I3,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="4">
-      <formula>AND(COUNTIF(E3:H3,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C3)))</formula>
+      <formula>AND(COUNTIF(F3:I3,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
     <cfRule type="expression" dxfId="1" priority="41">
-      <formula>COUNTIF(E30:H30,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F30:I30,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="42">
-      <formula>AND(COUNTIF(E30:H30,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C30)))</formula>
+      <formula>AND(COUNTIF(F30:I30,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C31">
     <cfRule type="expression" dxfId="1" priority="43">
-      <formula>COUNTIF(E31:H31,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F31:I31,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="44">
-      <formula>AND(COUNTIF(E31:H31,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C31)))</formula>
+      <formula>AND(COUNTIF(F31:I31,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
     <cfRule type="expression" dxfId="1" priority="45">
-      <formula>COUNTIF(E32:H32,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F32:I32,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="46">
-      <formula>AND(COUNTIF(E32:H32,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C32)))</formula>
+      <formula>AND(COUNTIF(F32:I32,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
     <cfRule type="expression" dxfId="1" priority="47">
-      <formula>COUNTIF(E33:H33,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F33:I33,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="48">
-      <formula>AND(COUNTIF(E33:H33,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C33)))</formula>
+      <formula>AND(COUNTIF(F33:I33,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
     <cfRule type="expression" dxfId="1" priority="49">
-      <formula>COUNTIF(E34:H34,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F34:I34,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="50">
-      <formula>AND(COUNTIF(E34:H34,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C34)))</formula>
+      <formula>AND(COUNTIF(F34:I34,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
     <cfRule type="expression" dxfId="1" priority="5">
-      <formula>COUNTIF(E4:H4,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F4:I4,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="6">
-      <formula>AND(COUNTIF(E4:H4,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C4)))</formula>
+      <formula>AND(COUNTIF(F4:I4,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
     <cfRule type="expression" dxfId="1" priority="7">
-      <formula>COUNTIF(E5:H5,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F5:I5,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="8">
-      <formula>AND(COUNTIF(E5:H5,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C5)))</formula>
+      <formula>AND(COUNTIF(F5:I5,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
     <cfRule type="expression" dxfId="1" priority="9">
-      <formula>COUNTIF(E6:H6,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F6:I6,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="10">
-      <formula>AND(COUNTIF(E6:H6,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C6)))</formula>
+      <formula>AND(COUNTIF(F6:I6,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
     <cfRule type="expression" dxfId="1" priority="11">
-      <formula>COUNTIF(E9:H9,"&lt;&gt;" &amp; "")&gt;0</formula>
+      <formula>COUNTIF(F9:I9,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="12">
-      <formula>AND(COUNTIF(E9:H9,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
+      <formula>AND(COUNTIF(F9:I9,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+      <formula1>"$/person,$/person/year"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4">
+      <formula1>"people/year,people"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10">
+      <formula1>"$/person,$/person/year"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11">
+      <formula1>"people/year,people"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
+      <formula1>"$/person,$/person/year"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18">
+      <formula1>"people/year,people"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24">
+      <formula1>"$/person,$/person/year"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B25">
+      <formula1>"people/year,people"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31">
+      <formula1>"$/person,$/person/year"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32">
+      <formula1>"people/year,people"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1915,19 +2058,19 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G1" s="2" t="str">
         <f>'Program targeting'!$B$3</f>
@@ -1959,10 +2102,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E2" s="5"/>
       <c r="G2" s="5"/>
@@ -1982,10 +2125,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E3" s="5"/>
       <c r="G3" s="5"/>
@@ -2005,10 +2148,10 @@
         <v>0</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E4" s="5"/>
       <c r="G4" s="6">
@@ -2028,10 +2171,10 @@
         <v>0</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E5" s="5"/>
       <c r="G5" s="6">
@@ -2044,19 +2187,19 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G7" s="2" t="str">
         <f>'Program targeting'!$B$3</f>
@@ -2088,10 +2231,10 @@
         <v>0</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E8" s="5"/>
       <c r="G8" s="5"/>
@@ -2111,10 +2254,10 @@
         <v>0</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E9" s="5"/>
       <c r="G9" s="5"/>
@@ -2134,10 +2277,10 @@
         <v>0</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E10" s="5"/>
       <c r="G10" s="5"/>
@@ -2157,10 +2300,10 @@
         <v>0</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E11" s="5"/>
       <c r="G11" s="5"/>
@@ -2173,19 +2316,19 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G13" s="2" t="str">
         <f>'Program targeting'!$B$3</f>
@@ -2217,10 +2360,10 @@
         <v>0</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E14" s="5"/>
       <c r="G14" s="5"/>
@@ -2240,10 +2383,10 @@
         <v>0</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E15" s="5"/>
       <c r="G15" s="5"/>
@@ -2263,10 +2406,10 @@
         <v>0</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E16" s="5"/>
       <c r="G16" s="5"/>
@@ -2286,10 +2429,10 @@
         <v>0</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E17" s="5"/>
       <c r="G17" s="5"/>
@@ -2302,19 +2445,19 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="E19" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G19" s="2" t="str">
         <f>'Program targeting'!$B$3</f>
@@ -2346,10 +2489,10 @@
         <v>0.15</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E20" s="5"/>
       <c r="G20" s="5"/>
@@ -2369,10 +2512,10 @@
         <v>0.15</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E21" s="5"/>
       <c r="G21" s="5"/>
@@ -2392,10 +2535,10 @@
         <v>0.15</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E22" s="5"/>
       <c r="G22" s="5"/>
@@ -2415,10 +2558,10 @@
         <v>0.15</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E23" s="5"/>
       <c r="G23" s="5"/>
@@ -2431,19 +2574,19 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G25" s="2" t="str">
         <f>'Program targeting'!$B$3</f>
@@ -2475,10 +2618,10 @@
         <v>0.2</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E26" s="5"/>
       <c r="G26" s="5"/>
@@ -2498,10 +2641,10 @@
         <v>0.2</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E27" s="5"/>
       <c r="G27" s="5"/>
@@ -2521,10 +2664,10 @@
         <v>0.2</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E28" s="5"/>
       <c r="G28" s="5"/>
@@ -2544,10 +2687,10 @@
         <v>0.2</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E29" s="5"/>
       <c r="G29" s="5"/>

</xml_diff>